<commit_message>
Historias del spring 2
</commit_message>
<xml_diff>
--- a/back/temp/sample.xlsx
+++ b/back/temp/sample.xlsx
@@ -397,17 +397,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C88"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1">
-        <v>3106</v>
+        <v>2101</v>
       </c>
       <c r="B1" t="str">
-        <v>Universidad De Prueba Apolo</v>
+        <v>Universidad Aspera</v>
       </c>
     </row>
     <row r="2">
@@ -423,7 +423,7 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="str">
         <v/>
@@ -434,18 +434,906 @@
     </row>
     <row r="4">
       <c r="A4">
+        <v>3106</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Universidad De Prueba Apolo</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Número</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Nombre participante</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Correo participante</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
         <v>6</v>
       </c>
-      <c r="B4" t="str">
-        <v/>
-      </c>
-      <c r="C4" t="str">
+      <c r="B6" t="str">
+        <v/>
+      </c>
+      <c r="C6" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>3117</v>
+      </c>
+      <c r="B7" t="str">
+        <v>asdasdasd</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Número</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Nombre participante</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Correo participante</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" t="str">
+        <v/>
+      </c>
+      <c r="C9" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" t="str">
+        <v/>
+      </c>
+      <c r="C10" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11" t="str">
+        <v/>
+      </c>
+      <c r="C11" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12" t="str">
+        <v/>
+      </c>
+      <c r="C12" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13" t="str">
+        <v/>
+      </c>
+      <c r="C13" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14" t="str">
+        <v/>
+      </c>
+      <c r="C14" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>8</v>
+      </c>
+      <c r="B15" t="str">
+        <v/>
+      </c>
+      <c r="C15" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>9</v>
+      </c>
+      <c r="B16" t="str">
+        <v/>
+      </c>
+      <c r="C16" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>10</v>
+      </c>
+      <c r="B17" t="str">
+        <v/>
+      </c>
+      <c r="C17" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <v>11</v>
+      </c>
+      <c r="B18" t="str">
+        <v/>
+      </c>
+      <c r="C18" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
+        <v>12</v>
+      </c>
+      <c r="B19" t="str">
+        <v/>
+      </c>
+      <c r="C19" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20">
+        <v>3118</v>
+      </c>
+      <c r="B20" t="str">
+        <v>Universidad Piola</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>Número</v>
+      </c>
+      <c r="B21" t="str">
+        <v>Nombre participante</v>
+      </c>
+      <c r="C21" t="str">
+        <v>Correo participante</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" t="str">
+        <v/>
+      </c>
+      <c r="C22" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23" t="str">
+        <v/>
+      </c>
+      <c r="C23" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24" t="str">
+        <v/>
+      </c>
+      <c r="C24" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25">
+        <v>4</v>
+      </c>
+      <c r="B25" t="str">
+        <v/>
+      </c>
+      <c r="C25" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26">
+        <v>5</v>
+      </c>
+      <c r="B26" t="str">
+        <v/>
+      </c>
+      <c r="C26" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
+        <v>6</v>
+      </c>
+      <c r="B27" t="str">
+        <v/>
+      </c>
+      <c r="C27" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28">
+        <v>7</v>
+      </c>
+      <c r="B28" t="str">
+        <v/>
+      </c>
+      <c r="C28" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29">
+        <v>8</v>
+      </c>
+      <c r="B29" t="str">
+        <v/>
+      </c>
+      <c r="C29" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30">
+        <v>9</v>
+      </c>
+      <c r="B30" t="str">
+        <v/>
+      </c>
+      <c r="C30" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31">
+        <v>10</v>
+      </c>
+      <c r="B31" t="str">
+        <v/>
+      </c>
+      <c r="C31" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32">
+        <v>11</v>
+      </c>
+      <c r="B32" t="str">
+        <v/>
+      </c>
+      <c r="C32" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33">
+        <v>12</v>
+      </c>
+      <c r="B33" t="str">
+        <v/>
+      </c>
+      <c r="C33" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34">
+        <v>13</v>
+      </c>
+      <c r="B34" t="str">
+        <v/>
+      </c>
+      <c r="C34" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
+        <v>14</v>
+      </c>
+      <c r="B35" t="str">
+        <v/>
+      </c>
+      <c r="C35" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36">
+        <v>15</v>
+      </c>
+      <c r="B36" t="str">
+        <v/>
+      </c>
+      <c r="C36" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37">
+        <v>3119</v>
+      </c>
+      <c r="B37" t="str">
+        <v>Prueba 1</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>Número</v>
+      </c>
+      <c r="B38" t="str">
+        <v>Nombre participante</v>
+      </c>
+      <c r="C38" t="str">
+        <v>Correo participante</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="B39" t="str">
+        <v/>
+      </c>
+      <c r="C39" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40">
+        <v>2</v>
+      </c>
+      <c r="B40" t="str">
+        <v/>
+      </c>
+      <c r="C40" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41">
+        <v>3120</v>
+      </c>
+      <c r="B41" t="str">
+        <v>Prueba 2</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>Número</v>
+      </c>
+      <c r="B42" t="str">
+        <v>Nombre participante</v>
+      </c>
+      <c r="C42" t="str">
+        <v>Correo participante</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43">
+        <v>1</v>
+      </c>
+      <c r="B43" t="str">
+        <v/>
+      </c>
+      <c r="C43" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44">
+        <v>2</v>
+      </c>
+      <c r="B44" t="str">
+        <v/>
+      </c>
+      <c r="C44" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45">
+        <v>3</v>
+      </c>
+      <c r="B45" t="str">
+        <v/>
+      </c>
+      <c r="C45" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46">
+        <v>3121</v>
+      </c>
+      <c r="B46" t="str">
+        <v>Prueba 1</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>Número</v>
+      </c>
+      <c r="B47" t="str">
+        <v>Nombre participante</v>
+      </c>
+      <c r="C47" t="str">
+        <v>Correo participante</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48">
+        <v>1</v>
+      </c>
+      <c r="B48" t="str">
+        <v/>
+      </c>
+      <c r="C48" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49">
+        <v>2</v>
+      </c>
+      <c r="B49" t="str">
+        <v/>
+      </c>
+      <c r="C49" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50">
+        <v>3122</v>
+      </c>
+      <c r="B50" t="str">
+        <v>Prueba 2</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>Número</v>
+      </c>
+      <c r="B51" t="str">
+        <v>Nombre participante</v>
+      </c>
+      <c r="C51" t="str">
+        <v>Correo participante</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52">
+        <v>1</v>
+      </c>
+      <c r="B52" t="str">
+        <v/>
+      </c>
+      <c r="C52" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53">
+        <v>2</v>
+      </c>
+      <c r="B53" t="str">
+        <v/>
+      </c>
+      <c r="C53" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54">
+        <v>3</v>
+      </c>
+      <c r="B54" t="str">
+        <v/>
+      </c>
+      <c r="C54" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55">
+        <v>3123</v>
+      </c>
+      <c r="B55" t="str">
+        <v>Prueba 3</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>Número</v>
+      </c>
+      <c r="B56" t="str">
+        <v>Nombre participante</v>
+      </c>
+      <c r="C56" t="str">
+        <v>Correo participante</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57">
+        <v>1</v>
+      </c>
+      <c r="B57" t="str">
+        <v/>
+      </c>
+      <c r="C57" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58">
+        <v>2</v>
+      </c>
+      <c r="B58" t="str">
+        <v/>
+      </c>
+      <c r="C58" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59">
+        <v>3</v>
+      </c>
+      <c r="B59" t="str">
+        <v/>
+      </c>
+      <c r="C59" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60">
+        <v>4</v>
+      </c>
+      <c r="B60" t="str">
+        <v/>
+      </c>
+      <c r="C60" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61">
+        <v>5</v>
+      </c>
+      <c r="B61" t="str">
+        <v/>
+      </c>
+      <c r="C61" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62">
+        <v>3124</v>
+      </c>
+      <c r="B62" t="str">
+        <v>Prueba 4</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>Número</v>
+      </c>
+      <c r="B63" t="str">
+        <v>Nombre participante</v>
+      </c>
+      <c r="C63" t="str">
+        <v>Correo participante</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64">
+        <v>1</v>
+      </c>
+      <c r="B64" t="str">
+        <v/>
+      </c>
+      <c r="C64" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65">
+        <v>2</v>
+      </c>
+      <c r="B65" t="str">
+        <v/>
+      </c>
+      <c r="C65" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66">
+        <v>3</v>
+      </c>
+      <c r="B66" t="str">
+        <v/>
+      </c>
+      <c r="C66" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67">
+        <v>4</v>
+      </c>
+      <c r="B67" t="str">
+        <v/>
+      </c>
+      <c r="C67" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68">
+        <v>5</v>
+      </c>
+      <c r="B68" t="str">
+        <v/>
+      </c>
+      <c r="C68" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69">
+        <v>3125</v>
+      </c>
+      <c r="B69" t="str">
+        <v>Prueba 5</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="str">
+        <v>Número</v>
+      </c>
+      <c r="B70" t="str">
+        <v>Nombre participante</v>
+      </c>
+      <c r="C70" t="str">
+        <v>Correo participante</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71">
+        <v>1</v>
+      </c>
+      <c r="B71" t="str">
+        <v/>
+      </c>
+      <c r="C71" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72">
+        <v>2</v>
+      </c>
+      <c r="B72" t="str">
+        <v/>
+      </c>
+      <c r="C72" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73">
+        <v>3</v>
+      </c>
+      <c r="B73" t="str">
+        <v/>
+      </c>
+      <c r="C73" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74">
+        <v>4</v>
+      </c>
+      <c r="B74" t="str">
+        <v/>
+      </c>
+      <c r="C74" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75">
+        <v>5</v>
+      </c>
+      <c r="B75" t="str">
+        <v/>
+      </c>
+      <c r="C75" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76">
+        <v>3126</v>
+      </c>
+      <c r="B76" t="str">
+        <v>Prueba 6</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v>Número</v>
+      </c>
+      <c r="B77" t="str">
+        <v>Nombre participante</v>
+      </c>
+      <c r="C77" t="str">
+        <v>Correo participante</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78">
+        <v>1</v>
+      </c>
+      <c r="B78" t="str">
+        <v/>
+      </c>
+      <c r="C78" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79">
+        <v>2</v>
+      </c>
+      <c r="B79" t="str">
+        <v/>
+      </c>
+      <c r="C79" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80">
+        <v>3</v>
+      </c>
+      <c r="B80" t="str">
+        <v/>
+      </c>
+      <c r="C80" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81">
+        <v>4</v>
+      </c>
+      <c r="B81" t="str">
+        <v/>
+      </c>
+      <c r="C81" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82">
+        <v>5</v>
+      </c>
+      <c r="B82" t="str">
+        <v/>
+      </c>
+      <c r="C82" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83">
+        <v>3127</v>
+      </c>
+      <c r="B83" t="str">
+        <v>Prueba 17</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="str">
+        <v>Número</v>
+      </c>
+      <c r="B84" t="str">
+        <v>Nombre participante</v>
+      </c>
+      <c r="C84" t="str">
+        <v>Correo participante</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85">
+        <v>2</v>
+      </c>
+      <c r="B85" t="str">
+        <v/>
+      </c>
+      <c r="C85" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86">
+        <v>3</v>
+      </c>
+      <c r="B86" t="str">
+        <v/>
+      </c>
+      <c r="C86" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87">
+        <v>4</v>
+      </c>
+      <c r="B87" t="str">
+        <v/>
+      </c>
+      <c r="C87" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88">
+        <v>5</v>
+      </c>
+      <c r="B88" t="str">
+        <v/>
+      </c>
+      <c r="C88" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C88"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>